<commit_message>
added osh demo analysis
</commit_message>
<xml_diff>
--- a/data/OSH-demo/metadata.xlsx
+++ b/data/OSH-demo/metadata.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="143" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62DC76A-170F-4A38-99C6-CB2BF7BC5FBE}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/vims-resazurin/data/OSH-demo/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB8C678-83E4-E141-85E6-483258AB17CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="23500" windowHeight="13840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="61">
   <si>
     <t>date</t>
   </si>
@@ -205,13 +210,22 @@
   </si>
   <si>
     <t>E08</t>
+  </si>
+  <si>
+    <t>Plate1</t>
+  </si>
+  <si>
+    <t>Plate2</t>
+  </si>
+  <si>
+    <t>Plate3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,11 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -284,9 +296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,7 +336,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -430,7 +442,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -572,7 +584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,19 +594,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A73"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -613,12 +625,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20260113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -633,12 +645,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20260113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -653,12 +665,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20260113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -673,12 +685,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20260113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -693,12 +705,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20260113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -713,12 +725,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20260113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -733,12 +745,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20260113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -753,12 +765,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20260113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -773,12 +785,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>20260113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -790,12 +802,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>20260113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -807,12 +819,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20260113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -824,12 +836,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20260113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -841,12 +853,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>20260113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -858,12 +870,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>20260113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -875,12 +887,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20260113</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -892,12 +904,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>20260113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -909,12 +921,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>20260113</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -929,12 +941,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>20260113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
@@ -949,12 +961,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20260113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -969,12 +981,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20260113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -989,12 +1001,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20260113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
@@ -1009,12 +1021,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>20260113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
@@ -1029,12 +1041,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20260113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -1049,12 +1061,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>20260113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
       </c>
       <c r="C25" t="s">
         <v>33</v>
@@ -1069,12 +1081,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>20260113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -1086,12 +1098,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>20260113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1103,12 +1115,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>20260113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
@@ -1120,12 +1132,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>20260113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
@@ -1137,12 +1149,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>20260113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
@@ -1154,12 +1166,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>20260113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -1171,12 +1183,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>20260113</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
       </c>
       <c r="C32" t="s">
         <v>40</v>
@@ -1188,12 +1200,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20260113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
@@ -1205,12 +1217,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>20260113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -1225,12 +1237,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>20260113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
@@ -1245,12 +1257,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>20260113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
       </c>
       <c r="C36" t="s">
         <v>19</v>
@@ -1265,12 +1277,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>20260113</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
@@ -1285,12 +1297,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>20260113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
@@ -1305,12 +1317,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>20260113</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
       </c>
       <c r="C39" t="s">
         <v>22</v>
@@ -1325,12 +1337,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>20260113</v>
+      </c>
+      <c r="B40" t="s">
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
@@ -1345,12 +1357,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>20260113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>24</v>
@@ -1365,12 +1377,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B42">
-        <v>2</v>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>20260113</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
       </c>
       <c r="C42" t="s">
         <v>42</v>
@@ -1385,12 +1397,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>20260113</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
       </c>
       <c r="C43" t="s">
         <v>43</v>
@@ -1405,12 +1417,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>20260113</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
@@ -1425,12 +1437,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B45">
-        <v>2</v>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>20260113</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>45</v>
@@ -1445,12 +1457,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20260113</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
       </c>
       <c r="C46" t="s">
         <v>46</v>
@@ -1465,12 +1477,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>20260113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>59</v>
       </c>
       <c r="C47" t="s">
         <v>47</v>
@@ -1485,12 +1497,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B48">
-        <v>2</v>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>20260113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>59</v>
       </c>
       <c r="C48" t="s">
         <v>48</v>
@@ -1505,12 +1517,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>20260113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
       </c>
       <c r="C49" t="s">
         <v>49</v>
@@ -1525,12 +1537,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>20260113</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -1545,12 +1557,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20260113</v>
+      </c>
+      <c r="B51" t="s">
+        <v>60</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -1565,12 +1577,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>20260113</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
@@ -1585,12 +1597,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>20260113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>60</v>
       </c>
       <c r="C53" t="s">
         <v>11</v>
@@ -1605,12 +1617,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>20260113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
       </c>
       <c r="C54" t="s">
         <v>12</v>
@@ -1625,12 +1637,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>20260113</v>
+      </c>
+      <c r="B55" t="s">
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
@@ -1645,12 +1657,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B56">
-        <v>3</v>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>20260113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -1665,12 +1677,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B57">
-        <v>3</v>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>20260113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
@@ -1685,12 +1697,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B58">
-        <v>3</v>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>20260113</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -1702,12 +1714,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B59">
-        <v>3</v>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>20260113</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
       </c>
       <c r="C59" t="s">
         <v>27</v>
@@ -1719,12 +1731,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B60">
-        <v>3</v>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>20260113</v>
+      </c>
+      <c r="B60" t="s">
+        <v>60</v>
       </c>
       <c r="C60" t="s">
         <v>28</v>
@@ -1736,12 +1748,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B61">
-        <v>3</v>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>20260113</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
       </c>
       <c r="C61" t="s">
         <v>29</v>
@@ -1753,12 +1765,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B62">
-        <v>3</v>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>20260113</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
       </c>
       <c r="C62" t="s">
         <v>30</v>
@@ -1770,12 +1782,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>20260113</v>
+      </c>
+      <c r="B63" t="s">
+        <v>60</v>
       </c>
       <c r="C63" t="s">
         <v>31</v>
@@ -1787,12 +1799,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B64">
-        <v>3</v>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>20260113</v>
+      </c>
+      <c r="B64" t="s">
+        <v>60</v>
       </c>
       <c r="C64" t="s">
         <v>32</v>
@@ -1804,12 +1816,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B65">
-        <v>3</v>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>20260113</v>
+      </c>
+      <c r="B65" t="s">
+        <v>60</v>
       </c>
       <c r="C65" t="s">
         <v>33</v>
@@ -1821,12 +1833,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B66">
-        <v>3</v>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>20260113</v>
+      </c>
+      <c r="B66" t="s">
+        <v>60</v>
       </c>
       <c r="C66" t="s">
         <v>50</v>
@@ -1841,12 +1853,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B67">
-        <v>3</v>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>20260113</v>
+      </c>
+      <c r="B67" t="s">
+        <v>60</v>
       </c>
       <c r="C67" t="s">
         <v>51</v>
@@ -1861,12 +1873,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B68">
-        <v>3</v>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>20260113</v>
+      </c>
+      <c r="B68" t="s">
+        <v>60</v>
       </c>
       <c r="C68" t="s">
         <v>52</v>
@@ -1881,12 +1893,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B69">
-        <v>3</v>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>20260113</v>
+      </c>
+      <c r="B69" t="s">
+        <v>60</v>
       </c>
       <c r="C69" t="s">
         <v>53</v>
@@ -1901,12 +1913,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B70">
-        <v>3</v>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>20260113</v>
+      </c>
+      <c r="B70" t="s">
+        <v>60</v>
       </c>
       <c r="C70" t="s">
         <v>54</v>
@@ -1921,12 +1933,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B71">
-        <v>3</v>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>20260113</v>
+      </c>
+      <c r="B71" t="s">
+        <v>60</v>
       </c>
       <c r="C71" t="s">
         <v>55</v>
@@ -1941,12 +1953,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B72">
-        <v>3</v>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>20260113</v>
+      </c>
+      <c r="B72" t="s">
+        <v>60</v>
       </c>
       <c r="C72" t="s">
         <v>56</v>
@@ -1961,12 +1973,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="3">
-        <v>20260113</v>
-      </c>
-      <c r="B73">
-        <v>3</v>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>20260113</v>
+      </c>
+      <c r="B73" t="s">
+        <v>60</v>
       </c>
       <c r="C73" t="s">
         <v>57</v>

</xml_diff>